<commit_message>
pbmc with new essential data
</commit_message>
<xml_diff>
--- a/template_examples/plasma_template.xlsx
+++ b/template_examples/plasma_template.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCD24CE-BD71-8D48-8DC8-AFE536D6A68E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32000" yWindow="2440" windowWidth="30360" windowHeight="16140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
     <sheet name="Essential Patient Data" sheetId="2" r:id="rId2"/>
     <sheet name="Samples" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,12 +30,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -60,7 +61,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -86,7 +87,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assay and sample type used. Example: Green-top tube - Plasma (Olink).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -95,11 +109,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assay and sample type used. Example: Green-top tube - Plasma (Olink).</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="0">
+          <t>The number corresponding to the batch sent for this assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -108,11 +122,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The number corresponding to the batch sent for this assay.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0">
+          <t>Box identifier for samples, if sample shipment container includes multiple boxes for each sample/assay type.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -121,11 +135,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Box identifier for samples, if sample shipment container includes multiple boxes for each sample/assay type.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0">
+          <t>Assay run number for samples received.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -134,11 +148,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assay run number for samples received.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0">
+          <t>Courier utilized for shipment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -147,11 +161,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier utilized for shipment.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0">
+          <t>Air bill number assigned to shipment. Example: 4567788343.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -160,11 +174,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Air bill number assigned to shipment. Example: 4567788343.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
+          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -173,11 +187,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Courier account number to pay for shipping if available. Example: 45465732.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B13" authorId="0">
+          <t>Type of shipment made.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -186,11 +200,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of shipment made.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B14" authorId="0">
+          <t>Date of shipment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -199,11 +213,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of shipment.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B15" authorId="0">
+          <t>Date of reciept.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -212,11 +226,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of reciept.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B16" authorId="0">
+          <t>Count of specimen(s) distributed by site.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -225,11 +239,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Count of specimen(s) distributed by site.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B17" authorId="0">
+          <t>Number of Sample(s) Received in Good Condition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -238,11 +252,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of Sample(s) Received in Good Condition.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B18" authorId="0">
+          <t>Number of pathology report(s) received.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -251,24 +265,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Number of pathology report(s) received.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B19" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Shipping from [free text: person or organization, address, phone number, email address.]</t>
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -286,12 +287,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -304,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -317,7 +318,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Descritpion of the topography category. e.g LUNG AND BRONCHUS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ICD-0-3 topography site code from which a specimen was isolated. e.g. C34.1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -326,11 +353,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Descritpion of the topography category. e.g LUNG AND BRONCHUS</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0">
+          <t>ICD-0-3 site code description. e.g. Upper lobe, lung</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -339,11 +366,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 topography site code from which a specimen was isolated. e.g. C34.1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="0">
+          <t>ICD-0-3 code for histology and behavior. e.g. 9665/3</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -352,11 +379,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 site code description. e.g. Upper lobe, lung</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G2" authorId="0">
+          <t>ICD-0-3 histology and behavior code description. e.g. Hodgkin lymphoma, nod. scler., grade 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -365,37 +392,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>ICD-0-3 code for histology and behavior. e.g. 9665/3</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>ICD-0-3 histology and behavior code description. e.g. Hodgkin lymphoma, nod. scler., grade 1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Identifies the gender of the participant.</t>
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -409,7 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -428,12 +429,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -446,7 +447,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -459,7 +460,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -472,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -485,7 +486,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Aliquot identifier assigned by the biorepository site: EA123-45-1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formated as CM-????-????-??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -494,11 +521,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Aliquot identifier assigned by the biorepository site: EA123-45-1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G2" authorId="0">
+          <t>Categorical description of timepoint at which the sample was taken.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -507,11 +534,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formated as CM-????-????-??</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H2" authorId="0">
+          <t>The type of material submitted - tumor/normal/etc</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -520,11 +547,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Categorical description of timepoint at which the sample was taken.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I2" authorId="0">
+          <t>Date of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -533,11 +560,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The type of material submitted - tumor/normal/etc</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J2" authorId="0">
+          <t>Time of blood collection.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -546,11 +573,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K2" authorId="0">
+          <t>Date of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -559,11 +586,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood collection.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L2" authorId="0">
+          <t>Time of blood processing.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -572,11 +599,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M2" authorId="0">
+          <t>Records if a sample processing (blood or tissue) is not compliant with protocol.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -585,11 +612,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Time of blood processing.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N2" authorId="0">
+          <t>Sample location within the shipping container. Example: A1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -598,11 +625,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Records if a sample processing (blood or tissue) is not compliant with protocol.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="O2" authorId="0">
+          <t>Type of sample sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -611,11 +638,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Sample location within the shipping container. Example: A1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P2" authorId="0">
+          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -624,11 +651,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Type of sample sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Q2" authorId="0">
+          <t>The format in which the sample was sent.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -637,11 +664,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates the specimen source of the sample shipped. Example: Na Heparin blood draw aliquots (2 of three), FFPE block #52</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="R2" authorId="0">
+          <t>Quantity of each aliquot shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -650,11 +677,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The format in which the sample was sent.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S2" authorId="0">
+          <t>Volume of aliquot shipped.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -663,11 +690,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Quantity of each aliquot shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="T2" authorId="0">
+          <t>The unit of biological material from this sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -676,11 +703,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Volume of aliquot shipped.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="U2" authorId="0">
+          <t>Receiving site indicates how much material was used for assay purposes.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="W2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -689,11 +716,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The unit of biological material from this sample.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V2" authorId="0">
+          <t>Units for the amount of material used; should be the same value as Specimen Analyte units.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -702,11 +729,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material was used for assay purposes.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="W2" authorId="0">
+          <t>Receiving site indicates how much material remains after assay use.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -715,11 +742,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Units for the amount of material used; should be the same value as Specimen Analyte units.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="X2" authorId="0">
+          <t>Units for the amount of material remaining.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Z2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -728,11 +755,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Receiving site indicates how much material remains after assay use.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Y2" authorId="0">
+          <t>Final status of aliquot after QC and pathology review.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -741,11 +768,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Units for the amount of material remaining.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="Z2" authorId="0">
+          <t>Final status of sample after QC and pathology review.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -754,11 +781,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of aliquot after QC and pathology review.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AA2" authorId="0">
+          <t>Indication if sample replacement is/was requested.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -767,37 +794,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AB2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Indication if sample replacement is/was requested.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AC2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t>Indication if sample was sent to another location or returned back to biorepository.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="0">
+    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -815,7 +816,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="102">
   <si>
     <t>#t</t>
   </si>
@@ -973,9 +974,6 @@
     <t>TYPE OF SAMPLE</t>
   </si>
   <si>
-    <t>SAMPLE_COLLECTION_PROCEDURE</t>
-  </si>
-  <si>
     <t>TYPE OF PRIMARY CONTAINER</t>
   </si>
   <si>
@@ -1115,13 +1113,22 @@
   </si>
   <si>
     <t>Neoplasm, malignant</t>
+  </si>
+  <si>
+    <t>ship from</t>
+  </si>
+  <si>
+    <t>ship to</t>
+  </si>
+  <si>
+    <t>SAMPLE COLLECTION PROCEDURE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1140,6 +1147,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1236,6 +1249,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1527,11 +1543,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F223"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1552,7 +1568,7 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1560,13 +1576,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1574,13 +1590,13 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1588,13 +1604,13 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1602,13 +1618,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1616,13 +1632,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1636,7 +1652,7 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1650,7 +1666,7 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1664,7 +1680,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1672,13 +1688,13 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1692,7 +1708,7 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1706,7 +1722,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1714,13 +1730,13 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1734,7 +1750,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1764,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1756,13 +1772,13 @@
         <v>17</v>
       </c>
       <c r="C16" s="2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1770,13 +1786,13 @@
         <v>18</v>
       </c>
       <c r="C17" s="2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1784,35 +1800,35 @@
         <v>19</v>
       </c>
       <c r="C18" s="2">
-        <v>123</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2">
-        <v>123</v>
+      <c r="C19" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2">
-        <v>123</v>
+      <c r="C20" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -2827,21 +2843,18 @@
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C15">
-      <formula1>AND(ISNUMBER(C15),LEFT(CELL("format",C15),1)="D")</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2850,11 +2863,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2863,7 +2876,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>24</v>
       </c>
@@ -2920,34 +2933,34 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" t="s">
         <v>91</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>92</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>93</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>94</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3" t="s">
         <v>95</v>
       </c>
-      <c r="H3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>96</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>97</v>
-      </c>
-      <c r="K3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -3951,28 +3964,28 @@
     <mergeCell ref="I1:K1"/>
   </mergeCells>
   <dataValidations count="8">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"ACCESSORY SINUS, NOS,ADRENAL GLANDS,ANAL CANAL &amp; ANUS,APPENDIX,BASE OF TONGUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"C00,C00.0,C00.1,C00.2,C00.3,C00.4,C00.5,C00.6,C00.8,C00.9,C01,C01.9"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3:F202" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"LIP,External upper lip,External lower lip,External lip, NOS,Mucosa of upper lip,Mucosa of lower lip,Mucosa of lip, NOS,Commissure of lip,Overlapping lesion of lip,Lip, NOS"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G202" xr:uid="{00000000-0002-0000-0100-000003000000}">
       <formula1>"8000/3,8001/3,8002/3,8003/3,8004/3,8005/3,8010/2,8010/3,8011/3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H4:H202" xr:uid="{00000000-0002-0000-0100-000004000000}">
       <formula1>"Neoplasm, malignant,Tumor cells, malignant,Malignant tumor, small cell type,Malignant tumor, giant cell type,Malignant tumor, spindle cell type,Malignant tumor, clear cell type"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000005000000}">
       <formula1>"Male,Female,Not Specified,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202" xr:uid="{00000000-0002-0000-0100-000006000000}">
       <formula1>"American Indian/Alaska Native,Asian,Black/African American,Native Hawaiian/Pacific Islander,White,Not Reported,Unknown,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K3:K202" xr:uid="{00000000-0002-0000-0100-000007000000}">
       <formula1>"Hispanic or Latino,Not Hispanic or Latino,Not reported,Unknown,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3982,11 +3995,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AD202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4080,46 +4093,46 @@
         <v>51</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="R2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
@@ -4130,25 +4143,25 @@
         <v>54321</v>
       </c>
       <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>70</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>71</v>
-      </c>
-      <c r="I3" t="s">
-        <v>72</v>
       </c>
       <c r="J3" s="4">
         <v>37174</v>
@@ -4163,19 +4176,19 @@
         <v>0.33333333333333331</v>
       </c>
       <c r="N3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O3">
         <v>123</v>
       </c>
       <c r="P3" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q3" t="s">
         <v>74</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>75</v>
-      </c>
-      <c r="R3" t="s">
-        <v>76</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4184,34 +4197,34 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="X3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z3" t="s">
         <v>78</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>79</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>80</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>81</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>82</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
@@ -5214,55 +5227,45 @@
     <mergeCell ref="B1:U1"/>
     <mergeCell ref="V1:AD1"/>
   </mergeCells>
-  <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
+  <dataValidations count="13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J3:J202 L3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J3:J202 L3:L202" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AND(ISNUMBER(J3:J202),LEFT(CELL("format",J3:J202),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K3:K202 M3">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K3:K202 M3:M202" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L4:L202">
-      <formula1>AND(ISNUMBER(L4:L203),LEFT(CELL("format",L4:L203),1)="D")</formula1>
-    </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M4:M202">
-      <formula1>0</formula1>
-      <formula2>0.999305555555555</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N3:N202" xr:uid="{00000000-0002-0000-0200-000005000000}">
       <formula1>"Compliant_processing,Noncompliant_tissue_fixation_24_to_36_hrs,Noncompliant_tissue_fixation_over_36_hrs,Noncompliant_blood_processing_ 24_to_48_hrs,Noncompliant_blood_processing_over_48_hrs,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:P202" xr:uid="{00000000-0002-0000-0200-000006000000}">
       <formula1>"Tumor Tissue,Normal Tissue,Skin Tissue,Blood,Bone Marrow,Cerebrospinal Fluid,Stool,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3:Q202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q3:Q202" xr:uid="{00000000-0002-0000-0200-000007000000}">
       <formula1>"Blood Draw,Excision,Core Biopsy,Punch Biopsy,Endoscopic Biopsy,Bone Marrow Core Biopsy,Bone Marrow Aspirate,Lumbar Puncture,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:R202" xr:uid="{00000000-0002-0000-0200-000008000000}">
       <formula1>"Sodium heparin,Blood specimen container with EDTA,Potassium EDTA,Streck Blood Collection Tube,Stool collection container with DNA stabilizer,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U202" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W202 Y3:Y202" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y202">
-      <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{00000000-0002-0000-0200-00000C000000}">
       <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202" xr:uid="{00000000-0002-0000-0200-00000D000000}">
       <formula1>"Pass,Fail,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB202" xr:uid="{00000000-0002-0000-0200-00000E000000}">
       <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC3:AC202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC3:AC202" xr:uid="{00000000-0002-0000-0200-00000F000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
moved QUALITY OF SHIPMENT from sample to shipment
</commit_message>
<xml_diff>
--- a/template_examples/plasma_template.xlsx
+++ b/template_examples/plasma_template.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CCD24CE-BD71-8D48-8DC8-AFE536D6A68E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4900AF-ADC9-1F4F-B635-C7E0AAE30854}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15960" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="720" windowWidth="24280" windowHeight="13280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,6 @@
     <sheet name="Samples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -92,7 +84,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -213,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of reciept.</t>
+          <t>Date of receipt.</t>
         </r>
       </text>
     </comment>
@@ -226,11 +218,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Final status of aliquot after QC and pathology review.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Count of specimen(s) distributed by site.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -243,7 +248,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -256,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -269,7 +274,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -323,7 +328,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -336,7 +341,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -491,7 +496,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -504,7 +509,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -755,7 +760,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of aliquot after QC and pathology review.</t>
+          <t>Final status of sample after QC and pathology review.</t>
         </r>
       </text>
     </comment>
@@ -768,7 +773,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Final status of sample after QC and pathology review.</t>
+          <t>Indication if sample replacement is/was requested.</t>
         </r>
       </text>
     </comment>
@@ -781,24 +786,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indication if sample replacement is/was requested.</t>
+          <t>Indication if sample was sent to another location or returned back to biorepository.</t>
         </r>
       </text>
     </comment>
     <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Indication if sample was sent to another location or returned back to biorepository.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -816,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="102">
   <si>
     <t>#t</t>
   </si>
@@ -869,6 +861,9 @@
     <t>DATE RECIEVED</t>
   </si>
   <si>
+    <t>QUALITY OF SHIPMENT</t>
+  </si>
+  <si>
     <t>NUM OF SAMPLES SHIPPED</t>
   </si>
   <si>
@@ -974,6 +969,9 @@
     <t>TYPE OF SAMPLE</t>
   </si>
   <si>
+    <t>SAMPLE COLLECTION PROCEDURE</t>
+  </si>
+  <si>
     <t>TYPE OF PRIMARY CONTAINER</t>
   </si>
   <si>
@@ -998,9 +996,6 @@
     <t>MATERIAL REMAINING UNITS</t>
   </si>
   <si>
-    <t>QUALITY OF SHIPMENT</t>
-  </si>
-  <si>
     <t>QUALITY OF SAMPLE</t>
   </si>
   <si>
@@ -1013,21 +1008,78 @@
     <t>COMMENTS</t>
   </si>
   <si>
+    <t>TEST123</t>
+  </si>
+  <si>
+    <t>TEST123_plasma</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Assay-1</t>
+  </si>
+  <si>
+    <t>Not sure about this value</t>
+  </si>
+  <si>
+    <t>USPS</t>
+  </si>
+  <si>
+    <t>Frozen (Dry Ice)</t>
+  </si>
+  <si>
+    <t>Specimen shipment received in good condition</t>
+  </si>
+  <si>
+    <t>ship from</t>
+  </si>
+  <si>
+    <t>ship to</t>
+  </si>
+  <si>
+    <t>CM-TEST-PA01-A1</t>
+  </si>
+  <si>
+    <t>Tumor_Pre_1</t>
+  </si>
+  <si>
+    <t>ADRENAL GLANDS</t>
+  </si>
+  <si>
+    <t>C00.2</t>
+  </si>
+  <si>
+    <t>External lower lip</t>
+  </si>
+  <si>
+    <t>8003/3</t>
+  </si>
+  <si>
+    <t>Neoplasm, malignant</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>Black/African American</t>
+  </si>
+  <si>
+    <t>Not Hispanic or Latino</t>
+  </si>
+  <si>
+    <t>RESPONDER</t>
+  </si>
+  <si>
     <t>ARM B</t>
   </si>
   <si>
-    <t>RESPONDER</t>
-  </si>
-  <si>
     <t>TRIALGROUP 1</t>
   </si>
   <si>
     <t>BIOBANK 1</t>
   </si>
   <si>
-    <t>CM-TEST-PA01-A1</t>
-  </si>
-  <si>
     <t>Level_1_starting</t>
   </si>
   <si>
@@ -1052,9 +1104,6 @@
     <t>Milliliters</t>
   </si>
   <si>
-    <t>Specimen shipment received in poor condition</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -1065,70 +1114,13 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>TEST123</t>
-  </si>
-  <si>
-    <t>OLINK-123</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Assay-1</t>
-  </si>
-  <si>
-    <t>Not sure about this value</t>
-  </si>
-  <si>
-    <t>USPS</t>
-  </si>
-  <si>
-    <t>Frozen (Dry Ice)</t>
-  </si>
-  <si>
-    <t>Tumor_Pre_1</t>
-  </si>
-  <si>
-    <t>ADRENAL GLANDS</t>
-  </si>
-  <si>
-    <t>C00.2</t>
-  </si>
-  <si>
-    <t>External lower lip</t>
-  </si>
-  <si>
-    <t>8003/3</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
-    <t>Black/African American</t>
-  </si>
-  <si>
-    <t>Not Hispanic or Latino</t>
-  </si>
-  <si>
-    <t>Neoplasm, malignant</t>
-  </si>
-  <si>
-    <t>ship from</t>
-  </si>
-  <si>
-    <t>ship to</t>
-  </si>
-  <si>
-    <t>SAMPLE COLLECTION PROCEDURE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1147,12 +1139,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1232,14 +1218,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1303,9 +1289,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1333,14 +1319,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1368,6 +1371,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1544,10 +1564,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F223"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1556,19 +1576,19 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1576,13 +1596,13 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1590,7 +1610,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1604,7 +1624,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1618,7 +1638,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1632,7 +1652,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1688,7 +1708,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1730,7 +1750,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
@@ -1743,7 +1763,7 @@
       <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>37174</v>
       </c>
       <c r="D14" s="2"/>
@@ -1757,22 +1777,22 @@
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>37539</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
+      <c r="C16" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1813,8 +1833,8 @@
       <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>99</v>
+      <c r="C19" s="2">
+        <v>1</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1828,16 +1848,25 @@
         <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -1846,1015 +1875,1023 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{10701B2F-C0C6-C44B-B423-FC17011593C8}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{D988D5F7-140E-4F4C-A49A-7DEDEB31A676}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D1688E35-AE77-744D-B349-B1CF85F2138A}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{EDA8B141-47CD-8E44-861D-17AE10001EE5}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{C933B8BB-D59C-C14D-AC0F-32A5E5DD89A0}">
+      <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2866,8 +2903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2878,1084 +2915,1084 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="H3" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I3" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="K3" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3996,10 +4033,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AD202"/>
+  <dimension ref="A1:AC202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4008,187 +4045,183 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AD1" s="7"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AC2" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>54321</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="H3" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
-      </c>
-      <c r="J3" s="4">
+        <v>91</v>
+      </c>
+      <c r="J3" s="6">
         <v>37174</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K3" s="7">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="6">
         <v>37174</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="7">
         <v>0.33333333333333331</v>
       </c>
       <c r="N3" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="O3">
         <v>123</v>
       </c>
       <c r="P3" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="Q3" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="R3" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4197,1044 +4230,1041 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="X3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="Z3" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="AA3" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="AB3" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="AC3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:U1"/>
-    <mergeCell ref="V1:AD1"/>
+    <mergeCell ref="V1:AC1"/>
   </mergeCells>
-  <dataValidations count="13">
+  <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="J3:J202 L3:L202" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="L3:L202 J3:J202" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>AND(ISNUMBER(J3:J202),LEFT(CELL("format",J3:J202),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="K3:K202 M3:M202" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="time" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter time in format hh:mm" sqref="M3:M202 K3:K202" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
       <formula2>0.999305555555555</formula2>
     </dataValidation>
@@ -5253,19 +5283,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U3:U202" xr:uid="{00000000-0002-0000-0200-000009000000}">
       <formula1>"Microliter,Milliliter,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W3:W202 Y3:Y202" xr:uid="{00000000-0002-0000-0200-00000A000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y3:Y202 W3:W202" xr:uid="{00000000-0002-0000-0200-00000A000000}">
       <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{00000000-0002-0000-0200-00000C000000}">
-      <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
+      <formula1>"Pass,Fail,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202" xr:uid="{00000000-0002-0000-0200-00000D000000}">
-      <formula1>"Pass,Fail,Not Reported,Other"</formula1>
+      <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB202" xr:uid="{00000000-0002-0000-0200-00000E000000}">
-      <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC3:AC202" xr:uid="{00000000-0002-0000-0200-00000F000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
examples/plasma_template update with new column
</commit_message>
<xml_diff>
--- a/template_examples/plasma_template.xlsx
+++ b/template_examples/plasma_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B4900AF-ADC9-1F4F-B635-C7E0AAE30854}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A086E6B-85B9-5540-B13D-F0670746574C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="720" windowWidth="24280" windowHeight="13280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9820" yWindow="1560" windowWidth="24680" windowHeight="12460" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -760,11 +760,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Units for the amount of material remaining.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Final status of sample after QC and pathology review.</t>
         </r>
       </text>
     </comment>
-    <comment ref="AA2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
+    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -777,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AB2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
+    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -790,7 +803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AC2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
+    <comment ref="AD2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -808,7 +821,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="104">
   <si>
     <t>#t</t>
   </si>
@@ -996,6 +1009,9 @@
     <t>MATERIAL REMAINING UNITS</t>
   </si>
   <si>
+    <t>MATERIAL STORAGE CONDITION</t>
+  </si>
+  <si>
     <t>QUALITY OF SAMPLE</t>
   </si>
   <si>
@@ -1114,6 +1130,9 @@
   </si>
   <si>
     <t>Comment</t>
+  </si>
+  <si>
+    <t>(-20)oC</t>
   </si>
 </sst>
 </file>
@@ -1169,7 +1188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1203,15 +1222,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1220,6 +1258,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -1576,297 +1620,297 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+    </row>
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>1</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>123</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>123</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="6">
         <v>37174</v>
       </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="6">
         <v>37539</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>1</v>
       </c>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="C20" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -2878,19 +2922,19 @@
     <mergeCell ref="B1:F1"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{10701B2F-C0C6-C44B-B423-FC17011593C8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{78867842-8ABC-D849-9F66-AE59B4EEBCE0}">
       <formula1>"Assay-1,Assay-2,Assay-3,Assay-4,Assay-5,Assay-6,Assay-7,Assay-8,Assay-9,Assay-10,Assay-11,Assay-12,Assay-13,Assay-14,Assay-15,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{D988D5F7-140E-4F4C-A49A-7DEDEB31A676}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{0B86C6B9-1F94-0D45-B32F-A3CDF0B39D22}">
       <formula1>"FEDEX,USPS,UPC"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{D1688E35-AE77-744D-B349-B1CF85F2138A}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{573B7453-86F8-604B-AABE-4F637DC9ECAA}">
       <formula1>"Frozen (Dry Ice),Frozen (Dry Shipper),Ambient (Ice Pack),Ambient,Other"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{EDA8B141-47CD-8E44-861D-17AE10001EE5}">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter date in format mm/dd/yyyy" sqref="C14:C15" xr:uid="{2AEE5588-5CCE-C645-9113-401982D9F88A}">
       <formula1>AND(ISNUMBER(C14),LEFT(CELL("format",C14),1)="D")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{C933B8BB-D59C-C14D-AC0F-32A5E5DD89A0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C16" xr:uid="{9D70B1DA-E00E-2A40-A607-DAFEF1356309}">
       <formula1>"Specimen shipment received in good condition,Specimen shipment received in poor condition,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2903,7 +2947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K202"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="B3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2913,55 +2957,56 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2970,34 +3015,34 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="I3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="J3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -3996,9 +4041,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:C1"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D202" xr:uid="{00000000-0002-0000-0100-000000000000}">
@@ -4033,10 +4079,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AC202"/>
+  <dimension ref="A1:AD202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AB16" sqref="AB16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4045,130 +4091,134 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="M2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="N2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="Q2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="R2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="S2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="T2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="U2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="W2" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="X2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Y2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="Z2" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AA2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AC2" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -4176,52 +4226,52 @@
         <v>54321</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I3" t="s">
-        <v>91</v>
-      </c>
-      <c r="J3" s="6">
+        <v>92</v>
+      </c>
+      <c r="J3" s="7">
         <v>37174</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="7">
         <v>37174</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="8">
         <v>0.33333333333333331</v>
       </c>
       <c r="N3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="O3">
         <v>123</v>
       </c>
       <c r="P3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="Q3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="R3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S3">
         <v>1</v>
@@ -4230,22 +4280,22 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="V3">
         <v>1</v>
       </c>
       <c r="W3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="X3">
         <v>1</v>
       </c>
       <c r="Y3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="Z3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="AA3" t="s">
         <v>99</v>
@@ -4256,68 +4306,71 @@
       <c r="AC3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AD3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -5255,9 +5308,9 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:U1"/>
-    <mergeCell ref="V1:AC1"/>
+    <mergeCell ref="V1:AD1"/>
   </mergeCells>
-  <dataValidations count="12">
+  <dataValidations count="13">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Tumor,Normal,Metastasis"</formula1>
     </dataValidation>
@@ -5287,12 +5340,15 @@
       <formula1>"Microliters,Milliliters,Nanogram per Microliter,Milligram per Milliliter,Micrograms per Microliter,Cells per Vial,Not Reported,Other"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z3:Z202" xr:uid="{00000000-0002-0000-0200-00000C000000}">
+      <formula1>"RT,4oC,(-20)oC,(-80)oC,LN,Not Reported,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202" xr:uid="{00000000-0002-0000-0200-00000D000000}">
       <formula1>"Pass,Fail,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA3:AA202" xr:uid="{00000000-0002-0000-0200-00000D000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB202" xr:uid="{00000000-0002-0000-0200-00000E000000}">
       <formula1>"Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB3:AB202" xr:uid="{00000000-0002-0000-0200-00000E000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC3:AC202" xr:uid="{00000000-0002-0000-0200-00000F000000}">
       <formula1>"Sample Returned,Sample Sent to Another Lab,Sample received from CIMAC,Not Reported,Other"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updated enum values for diagnosis_verification
</commit_message>
<xml_diff>
--- a/template_examples/plasma_template.xlsx
+++ b/template_examples/plasma_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D8958B-B1CB-5D44-BB28-FF4F6521D7F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1CFC5A6-7482-7A46-B7A2-683B72563260}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9140" yWindow="7400" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9140" yWindow="7280" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -1111,7 +1111,7 @@
     <t>A6</t>
   </si>
   <si>
-    <t>verified</t>
+    <t>Local pathology review was not consistent</t>
   </si>
 </sst>
 </file>
@@ -2827,7 +2827,7 @@
   <dimension ref="A1:P202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
root prism object merger collision context
</commit_message>
<xml_diff>
--- a/template_examples/plasma_template.xlsx
+++ b/template_examples/plasma_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF861D42-81B0-0C49-B1B3-283F31064030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5B1332-B70F-C34C-8004-C6E0F8A35203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8820" yWindow="25140" windowWidth="21400" windowHeight="12740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shipment" sheetId="1" r:id="rId1"/>
@@ -589,7 +589,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -1652,7 +1652,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="354">
   <si>
     <t>#t</t>
   </si>
@@ -2615,24 +2615,12 @@
     <t>CTTTP01A1.00</t>
   </si>
   <si>
-    <t>TRIALGROUP 1</t>
-  </si>
-  <si>
-    <t>BIOBANK 1</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
     <t>Comment</t>
   </si>
   <si>
-    <t>TTTPP102</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 2</t>
-  </si>
-  <si>
     <t>CTTTP01A2.00</t>
   </si>
   <si>
@@ -2642,48 +2630,24 @@
     <t>No comment</t>
   </si>
   <si>
-    <t>TTTPP103</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 3</t>
-  </si>
-  <si>
     <t>CTTTP01A3.00</t>
   </si>
   <si>
     <t>A3</t>
   </si>
   <si>
-    <t>TTTPP201</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 4</t>
-  </si>
-  <si>
     <t>CTTTP02A1.00</t>
   </si>
   <si>
     <t>A4</t>
   </si>
   <si>
-    <t>TTTPP202</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 5</t>
-  </si>
-  <si>
     <t>CTTTP02A2.00</t>
   </si>
   <si>
     <t>A5</t>
   </si>
   <si>
-    <t>TTTPP203</t>
-  </si>
-  <si>
-    <t>TRIALGROUP 6</t>
-  </si>
-  <si>
     <t>CTTTP02A3.00</t>
   </si>
   <si>
@@ -2709,13 +2673,55 @@
   </si>
   <si>
     <t>Neoplasm, malignant</t>
+  </si>
+  <si>
+    <t>TTTPP1</t>
+  </si>
+  <si>
+    <t>TTTPP2</t>
+  </si>
+  <si>
+    <t>TTTPP1A1</t>
+  </si>
+  <si>
+    <t>TTTPP1A2</t>
+  </si>
+  <si>
+    <t>TTTPP1A3</t>
+  </si>
+  <si>
+    <t>TTTPP2A1</t>
+  </si>
+  <si>
+    <t>TTTPP2A2</t>
+  </si>
+  <si>
+    <t>TTTPP2A3</t>
+  </si>
+  <si>
+    <t>BIOBANK 1A1</t>
+  </si>
+  <si>
+    <t>BIOBANK 1A2</t>
+  </si>
+  <si>
+    <t>BIOBANK 1A3</t>
+  </si>
+  <si>
+    <t>BIOBANK 2A1</t>
+  </si>
+  <si>
+    <t>BIOBANK 2A2</t>
+  </si>
+  <si>
+    <t>BIOBANK 2A3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2742,6 +2748,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3174,14 +3186,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C218"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+    <sheetView topLeftCell="B6" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+    <col min="4" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
@@ -4485,10 +4499,10 @@
         <v>319</v>
       </c>
       <c r="E3" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="F3" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
       <c r="G3" t="s">
         <v>195</v>
@@ -4497,19 +4511,19 @@
         <v>219</v>
       </c>
       <c r="I3" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="J3" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="K3" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="L3" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
       <c r="M3" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="N3" t="s">
         <v>223</v>
@@ -5548,14 +5562,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:Y8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="30.6640625" customWidth="1"/>
+    <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" bestFit="1" customWidth="1"/>
+    <col min="26" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.2">
@@ -5681,13 +5718,13 @@
         <v>195</v>
       </c>
       <c r="E3" t="s">
-        <v>318</v>
+        <v>340</v>
       </c>
       <c r="F3" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="G3" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="H3" t="s">
         <v>319</v>
@@ -5696,7 +5733,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="K3" t="s">
         <v>261</v>
@@ -5741,7 +5778,7 @@
         <v>309</v>
       </c>
       <c r="Y3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.2">
@@ -5752,28 +5789,28 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="D4" t="s">
         <v>195</v>
       </c>
       <c r="E4" t="s">
-        <v>324</v>
+        <v>340</v>
       </c>
       <c r="F4" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="G4" t="s">
-        <v>321</v>
+        <v>349</v>
       </c>
       <c r="H4" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="I4">
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="K4" t="s">
         <v>261</v>
@@ -5818,7 +5855,7 @@
         <v>309</v>
       </c>
       <c r="Y4" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.2">
@@ -5835,22 +5872,22 @@
         <v>195</v>
       </c>
       <c r="E5" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="F5" t="s">
-        <v>330</v>
+        <v>344</v>
       </c>
       <c r="G5" t="s">
-        <v>321</v>
+        <v>350</v>
       </c>
       <c r="H5" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="I5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="K5" t="s">
         <v>261</v>
@@ -5909,22 +5946,22 @@
         <v>195</v>
       </c>
       <c r="E6" t="s">
-        <v>333</v>
+        <v>341</v>
       </c>
       <c r="F6" t="s">
-        <v>334</v>
+        <v>345</v>
       </c>
       <c r="G6" t="s">
-        <v>321</v>
+        <v>351</v>
       </c>
       <c r="H6" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="I6">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="K6" t="s">
         <v>261</v>
@@ -5977,28 +6014,28 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="D7" t="s">
         <v>195</v>
       </c>
       <c r="E7" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="F7" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
       <c r="G7" t="s">
-        <v>321</v>
+        <v>352</v>
       </c>
       <c r="H7" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="K7" t="s">
         <v>261</v>
@@ -6060,19 +6097,19 @@
         <v>341</v>
       </c>
       <c r="F8" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="G8" t="s">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c r="H8" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="K8" t="s">
         <v>261</v>
@@ -7093,6 +7130,7 @@
     <mergeCell ref="I1:P1"/>
     <mergeCell ref="Q1:Y1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="12">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C202" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Arm_A,Arm_B,Arm_C,Arm_D,Arm_E,Arm_F,Arm_G,Arm_H,Arm_I,Arm_X,Arm_Y,Arm_Z,Arm_1,Arm_2,EAY131-Z1D,NSCLC_A,NSCLC_B,NSCLC_C,CRC_A,CRC_B,Dose_A,Dose_B,Dose_C,Dose_D,Other,Not_reported"</formula1>

</xml_diff>